<commit_message>
Added Mimic Type column to raw data as there are non-mimics in the table.
</commit_message>
<xml_diff>
--- a/TraitTable/data/Raw data table.xlsx
+++ b/TraitTable/data/Raw data table.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="257">
   <si>
     <t>Unique I.D.</t>
   </si>
@@ -868,6 +868,15 @@
   </si>
   <si>
     <t>Faux-petiole length</t>
+  </si>
+  <si>
+    <t>Mimic Type</t>
+  </si>
+  <si>
+    <t>mimic</t>
+  </si>
+  <si>
+    <t>non-mimic</t>
   </si>
 </sst>
 </file>
@@ -1066,11 +1075,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3836,12 +3845,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ65"/>
+  <dimension ref="A1:AR65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3876,70 +3885,70 @@
     <col min="37" max="37" width="15.7109375" customWidth="1"/>
     <col min="38" max="38" width="8.7109375" customWidth="1"/>
     <col min="39" max="39" width="12" style="14" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="10.140625" customWidth="1"/>
-    <col min="43" max="43" width="148.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="10.140625" customWidth="1"/>
+    <col min="44" max="44" width="148.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:44" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21" t="s">
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21" t="s">
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21" t="s">
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21" t="s">
+      <c r="U1" s="22"/>
+      <c r="V1" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21" t="s">
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21" t="s">
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21" t="s">
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
     </row>
-    <row r="2" spans="1:43" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4054,7 +4063,7 @@
       <c r="AL2" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="AM2" s="22"/>
+      <c r="AM2" s="21"/>
       <c r="AN2" s="20" t="s">
         <v>253</v>
       </c>
@@ -4064,11 +4073,14 @@
       <c r="AP2" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="AR2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>163</v>
       </c>
@@ -4197,11 +4209,14 @@
         <f>SUM(H3,L3,P3,S3,U3,Y3,AC3,AG3,AK3)/9</f>
         <v>0.28723359276665167</v>
       </c>
-      <c r="AQ3" s="7" t="s">
+      <c r="AQ3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -4324,11 +4339,14 @@
         <f t="shared" ref="AL4:AL65" si="7">SUM(H4,L4,P4,S4,U4,Y4,AC4,AG4,AK4)/9</f>
         <v>0.15028042599664035</v>
       </c>
-      <c r="AQ4" s="7" t="s">
+      <c r="AQ4" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>216</v>
       </c>
@@ -4451,11 +4469,14 @@
         <f t="shared" si="7"/>
         <v>0.20672335778618092</v>
       </c>
-      <c r="AQ5" s="7" t="s">
+      <c r="AQ5" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>217</v>
       </c>
@@ -4578,11 +4599,14 @@
         <f t="shared" si="7"/>
         <v>0.17078653522686929</v>
       </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AQ6" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>218</v>
       </c>
@@ -4705,11 +4729,14 @@
         <f t="shared" si="7"/>
         <v>0.19426947519823598</v>
       </c>
-      <c r="AQ7" s="7" t="s">
+      <c r="AQ7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>219</v>
       </c>
@@ -4834,11 +4861,14 @@
         <f t="shared" si="7"/>
         <v>0.20793726647375921</v>
       </c>
-      <c r="AQ8" s="7" t="s">
+      <c r="AQ8" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR8" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
@@ -4961,11 +4991,14 @@
         <f t="shared" si="7"/>
         <v>0.15928661936163752</v>
       </c>
-      <c r="AQ9" s="7" t="s">
+      <c r="AQ9" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR9" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>220</v>
       </c>
@@ -5088,11 +5121,14 @@
         <f t="shared" si="7"/>
         <v>0.1476354167315426</v>
       </c>
-      <c r="AQ10" s="7" t="s">
+      <c r="AQ10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR10" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -5215,11 +5251,14 @@
         <f t="shared" si="7"/>
         <v>0.14773379099286454</v>
       </c>
-      <c r="AQ11" s="7" t="s">
+      <c r="AQ11" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR11" s="7" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -5340,11 +5379,14 @@
         <f t="shared" si="7"/>
         <v>5.8201058201058205E-2</v>
       </c>
-      <c r="AQ12" s="7" t="s">
+      <c r="AQ12" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR12" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>38</v>
       </c>
@@ -5467,11 +5509,14 @@
         <f t="shared" si="7"/>
         <v>0.12492238890960843</v>
       </c>
-      <c r="AQ13" s="7" t="s">
+      <c r="AQ13" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR13" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
@@ -5596,11 +5641,14 @@
         <f t="shared" si="7"/>
         <v>0.14817648290729901</v>
       </c>
-      <c r="AQ14" s="7" t="s">
+      <c r="AQ14" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR14" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
@@ -5725,11 +5773,14 @@
         <f t="shared" si="7"/>
         <v>0.15098343419477928</v>
       </c>
-      <c r="AQ15" s="7" t="s">
+      <c r="AQ15" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -5852,11 +5903,14 @@
         <f t="shared" si="7"/>
         <v>0.14812272508547963</v>
       </c>
-      <c r="AQ16" s="7" t="s">
+      <c r="AQ16" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR16" s="7" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>48</v>
       </c>
@@ -5979,11 +6033,14 @@
         <f t="shared" si="7"/>
         <v>0.15765730784446275</v>
       </c>
-      <c r="AQ17" s="7" t="s">
+      <c r="AQ17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR17" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
@@ -6106,11 +6163,14 @@
         <f t="shared" si="7"/>
         <v>0.16686714607589759</v>
       </c>
-      <c r="AQ18" s="7" t="s">
+      <c r="AQ18" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR18" s="7" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>221</v>
       </c>
@@ -6247,11 +6307,14 @@
         <f>AN19+AO19</f>
         <v>3.0019999999999998</v>
       </c>
-      <c r="AQ19" s="7" t="s">
+      <c r="AQ19" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR19" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>222</v>
       </c>
@@ -6376,11 +6439,14 @@
         <f t="shared" si="7"/>
         <v>0.21902219289291919</v>
       </c>
-      <c r="AQ20" s="7" t="s">
+      <c r="AQ20" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR20" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>223</v>
       </c>
@@ -6511,11 +6577,14 @@
         <f t="shared" si="7"/>
         <v>0.31992923278940083</v>
       </c>
-      <c r="AQ21" s="7" t="s">
+      <c r="AQ21" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR21" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -6638,11 +6707,14 @@
         <f t="shared" si="7"/>
         <v>0.18335623328860992</v>
       </c>
-      <c r="AQ22" s="7" t="s">
+      <c r="AQ22" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR22" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>61</v>
       </c>
@@ -6765,11 +6837,14 @@
         <f t="shared" si="7"/>
         <v>0.12369012509312692</v>
       </c>
-      <c r="AQ23" s="7" t="s">
+      <c r="AQ23" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR23" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>65</v>
       </c>
@@ -6892,11 +6967,14 @@
         <f t="shared" si="7"/>
         <v>0.18133809766995254</v>
       </c>
-      <c r="AQ24" s="7" t="s">
+      <c r="AQ24" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR24" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>67</v>
       </c>
@@ -7019,11 +7097,14 @@
         <f t="shared" si="7"/>
         <v>0.14487628310537384</v>
       </c>
-      <c r="AQ25" s="7" t="s">
+      <c r="AQ25" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR25" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>70</v>
       </c>
@@ -7146,11 +7227,14 @@
         <f t="shared" si="7"/>
         <v>0.13536262379596808</v>
       </c>
-      <c r="AQ26" s="7" t="s">
+      <c r="AQ26" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR26" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>73</v>
       </c>
@@ -7273,11 +7357,14 @@
         <f t="shared" si="7"/>
         <v>0.12976706691520126</v>
       </c>
-      <c r="AQ27" s="7" t="s">
+      <c r="AQ27" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR27" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>235</v>
       </c>
@@ -7400,11 +7487,14 @@
         <f t="shared" si="7"/>
         <v>0.13147689451226519</v>
       </c>
-      <c r="AQ28" s="7" t="s">
+      <c r="AQ28" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR28" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>76</v>
       </c>
@@ -7527,11 +7617,14 @@
         <f t="shared" si="7"/>
         <v>0.20679959207125032</v>
       </c>
-      <c r="AQ29" s="7" t="s">
+      <c r="AQ29" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR29" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>224</v>
       </c>
@@ -7654,11 +7747,14 @@
         <f t="shared" si="7"/>
         <v>0.15173846876808941</v>
       </c>
-      <c r="AQ30" s="7" t="s">
+      <c r="AQ30" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR30" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>81</v>
       </c>
@@ -7783,11 +7879,14 @@
         <f t="shared" si="7"/>
         <v>0.23230047454369382</v>
       </c>
-      <c r="AQ31" s="7" t="s">
+      <c r="AQ31" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR31" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>225</v>
       </c>
@@ -7916,11 +8015,14 @@
         <f t="shared" si="7"/>
         <v>0.19793806769243572</v>
       </c>
-      <c r="AQ32" s="7" t="s">
+      <c r="AQ32" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR32" s="7" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>226</v>
       </c>
@@ -8043,11 +8145,14 @@
         <f t="shared" si="7"/>
         <v>0.15569599218317542</v>
       </c>
-      <c r="AQ33" s="7" t="s">
+      <c r="AQ33" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR33" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>227</v>
       </c>
@@ -8188,11 +8293,14 @@
         <f>AN34+AO34</f>
         <v>5.9390000000000001</v>
       </c>
-      <c r="AQ34" s="7" t="s">
+      <c r="AQ34" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>92</v>
       </c>
@@ -8315,11 +8423,14 @@
         <f t="shared" si="7"/>
         <v>0.15737378931781348</v>
       </c>
-      <c r="AQ35" s="7" t="s">
+      <c r="AQ35" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR35" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>95</v>
       </c>
@@ -8442,11 +8553,14 @@
         <f t="shared" si="7"/>
         <v>0.14123907054862617</v>
       </c>
-      <c r="AQ36" s="7" t="s">
+      <c r="AQ36" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR36" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>98</v>
       </c>
@@ -8571,11 +8685,14 @@
         <f t="shared" si="7"/>
         <v>0.23384393627060543</v>
       </c>
-      <c r="AQ37" s="7" t="s">
+      <c r="AQ37" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR37" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>102</v>
       </c>
@@ -8698,11 +8815,14 @@
         <f t="shared" si="7"/>
         <v>0.19230442943500961</v>
       </c>
-      <c r="AQ38" s="7" t="s">
+      <c r="AQ38" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR38" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>109</v>
       </c>
@@ -8827,11 +8947,14 @@
         <f t="shared" si="7"/>
         <v>0.19577433494996693</v>
       </c>
-      <c r="AQ39" s="7" t="s">
+      <c r="AQ39" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR39" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>105</v>
       </c>
@@ -8956,11 +9079,14 @@
         <f t="shared" si="7"/>
         <v>0.19888590101920955</v>
       </c>
-      <c r="AQ40" s="7" t="s">
+      <c r="AQ40" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR40" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>111</v>
       </c>
@@ -9099,11 +9225,14 @@
         <f>AN41+AO41</f>
         <v>2.4009999999999998</v>
       </c>
-      <c r="AQ41" s="7" t="s">
+      <c r="AQ41" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR41" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>114</v>
       </c>
@@ -9242,11 +9371,14 @@
         <f>AN42+AO42</f>
         <v>2.085</v>
       </c>
-      <c r="AQ42" s="7" t="s">
+      <c r="AQ42" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR42" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>115</v>
       </c>
@@ -9385,11 +9517,14 @@
         <f>AN43+AO43</f>
         <v>2.3890000000000002</v>
       </c>
-      <c r="AQ43" s="7" t="s">
+      <c r="AQ43" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR43" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>118</v>
       </c>
@@ -9528,11 +9663,14 @@
         <f>AN44+AO44</f>
         <v>2.3540000000000001</v>
       </c>
-      <c r="AQ44" s="7" t="s">
+      <c r="AQ44" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR44" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>228</v>
       </c>
@@ -9673,11 +9811,14 @@
         <f>AN45+AO45</f>
         <v>1.9140000000000001</v>
       </c>
-      <c r="AQ45" s="7" t="s">
+      <c r="AQ45" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR45" s="7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>229</v>
       </c>
@@ -9808,11 +9949,14 @@
         <f t="shared" si="7"/>
         <v>0.29524033766371022</v>
       </c>
-      <c r="AQ46" s="7" t="s">
+      <c r="AQ46" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR46" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>230</v>
       </c>
@@ -9941,11 +10085,14 @@
         <f t="shared" si="7"/>
         <v>0.29203705407409614</v>
       </c>
-      <c r="AQ47" s="7" t="s">
+      <c r="AQ47" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR47" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>231</v>
       </c>
@@ -10086,11 +10233,14 @@
         <f>AN48+AO48</f>
         <v>3.931</v>
       </c>
-      <c r="AQ48" s="7" t="s">
+      <c r="AQ48" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR48" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>129</v>
       </c>
@@ -10231,11 +10381,14 @@
         <f>AN49+AO49</f>
         <v>3.2839999999999998</v>
       </c>
-      <c r="AQ49" s="7" t="s">
+      <c r="AQ49" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR49" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>131</v>
       </c>
@@ -10376,11 +10529,14 @@
         <f>AN50+AO50</f>
         <v>3.0910000000000002</v>
       </c>
-      <c r="AQ50" s="7" t="s">
+      <c r="AQ50" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR50" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>132</v>
       </c>
@@ -10511,11 +10667,14 @@
         <f t="shared" si="7"/>
         <v>0.30541824937445811</v>
       </c>
-      <c r="AQ51" s="7" t="s">
+      <c r="AQ51" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR51" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>135</v>
       </c>
@@ -10646,11 +10805,14 @@
         <f t="shared" si="7"/>
         <v>0.30524110064199328</v>
       </c>
-      <c r="AQ52" s="7" t="s">
+      <c r="AQ52" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR52" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>137</v>
       </c>
@@ -10777,11 +10939,14 @@
         <f t="shared" si="7"/>
         <v>0.25201964078691091</v>
       </c>
-      <c r="AQ53" s="7" t="s">
+      <c r="AQ53" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR53" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>126</v>
       </c>
@@ -10912,11 +11077,14 @@
         <f t="shared" si="7"/>
         <v>0.31957619422889144</v>
       </c>
-      <c r="AQ54" s="7" t="s">
+      <c r="AQ54" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR54" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>141</v>
       </c>
@@ -11045,11 +11213,14 @@
         <f t="shared" si="7"/>
         <v>0.33056684599376596</v>
       </c>
-      <c r="AQ55" s="7" t="s">
+      <c r="AQ55" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR55" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>243</v>
       </c>
@@ -11178,9 +11349,12 @@
         <f t="shared" si="7"/>
         <v>0.33121969677836166</v>
       </c>
-      <c r="AQ56" s="7"/>
+      <c r="AQ56" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR56" s="7"/>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>143</v>
       </c>
@@ -11321,11 +11495,14 @@
         <f>AN57+AO57</f>
         <v>2.2640000000000002</v>
       </c>
-      <c r="AQ57" s="7" t="s">
+      <c r="AQ57" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR57" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>145</v>
       </c>
@@ -11466,11 +11643,14 @@
         <f>AN58+AO58</f>
         <v>2.4989999999999997</v>
       </c>
-      <c r="AQ58" s="7" t="s">
+      <c r="AQ58" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR58" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>147</v>
       </c>
@@ -11601,11 +11781,14 @@
         <f t="shared" si="7"/>
         <v>0.33663997876332286</v>
       </c>
-      <c r="AQ59" s="7" t="s">
+      <c r="AQ59" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR59" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>149</v>
       </c>
@@ -11736,11 +11919,14 @@
         <f t="shared" si="7"/>
         <v>0.34077541009556284</v>
       </c>
-      <c r="AQ60" s="7" t="s">
+      <c r="AQ60" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR60" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>151</v>
       </c>
@@ -11881,11 +12067,14 @@
         <f>AN61+AO61</f>
         <v>3.927</v>
       </c>
-      <c r="AQ61" s="7" t="s">
+      <c r="AQ61" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR61" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>232</v>
       </c>
@@ -12008,11 +12197,14 @@
         <f t="shared" si="7"/>
         <v>0.13191525524033088</v>
       </c>
-      <c r="AQ62" s="7" t="s">
+      <c r="AQ62" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR62" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>154</v>
       </c>
@@ -12135,11 +12327,14 @@
         <f t="shared" si="7"/>
         <v>0.12721506069235311</v>
       </c>
-      <c r="AQ63" s="7" t="s">
+      <c r="AQ63" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR63" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>158</v>
       </c>
@@ -12262,11 +12457,14 @@
         <f t="shared" si="7"/>
         <v>0.16087854867901016</v>
       </c>
-      <c r="AQ64" s="7" t="s">
+      <c r="AQ64" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR64" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>159</v>
       </c>
@@ -12407,7 +12605,10 @@
         <f>AN65+AO65</f>
         <v>1.4500000000000002</v>
       </c>
-      <c r="AQ65" s="7" t="s">
+      <c r="AQ65" t="s">
+        <v>255</v>
+      </c>
+      <c r="AR65" s="7" t="s">
         <v>162</v>
       </c>
     </row>
@@ -12424,14 +12625,14 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:D3 M3:M16 AQ3:AQ7 M18:M25 AQ46 A4:C4 Y4:Y11 AG4:AG24 AB62 AB64 Z62 V62 Z64:Z65 V65:W65 AH48:AH49 AH54:AH55 AH62 AH64:AH65 AJ14 AF3:AG3 AJ3:AK3 AJ48:AJ49 AJ54:AJ55 AJ62 AJ64:AJ65 AJ19 AD49:AF49 AD54:AE55 AD62:AE62 AD65:AE65 Z3:Z5 AB4:AB5 AF4:AF5 V21:X21 AB21 AH3:AH9 AD7 AJ4:AJ9 N3:N25 O3:T20 V7:V11 Y13 AD8:AF12 AJ11:AJ12 V13 AD14:AF14 V15 AD16:AE16 AD19:AF21 V19 AJ21 O21:S21 V24 AD24:AF24 M27:N29 AQ9:AQ28 Z7:Z29 Y15:Y28 E22:L28 AI27:AI29 V27 AD27:AD28 E29 AD30 E31:F31 AB32 AJ31:AJ32 V32:X32 AD32:AF32 H32:L32 AD33 AH11:AH27 AG27 M31:N38 Z31:Z41 AQ30:AQ38 Y30:Y38 AI31:AI38 E33:F38 AB34 AD34:AF34 AJ34 AD37:AF37 AD35:AD36 V34:X38 V40:W41 AQ41 AD38:AD40 E44:F46 AB44:AB45 Z44:Z45 A5:D48 AH29:AH45 AJ41:AJ45 AD41:AE48 AF42:AF48 E47 Z47:Z49 AQ49 M44:N49 V44:X49 AI44:AI49 E48:F49 AB47:AB49 AK4:AK55 AC3:AC55 AA8:AA55 AG29:AG55 Y41:Y55 AQ51:AQ54 O22:T55 O57:T65 Y57:Y61 AG57:AG63 AA57:AA65 AC57:AC64 AK58:AK65 AQ62:AQ63 Y63:Y65 V64 AG65 AD64 V3:Y3 AD3:AE5 V4:X5 E3:L20 G21:L21 G29:L31 G33:L55 G57:L65">
+  <conditionalFormatting sqref="A3:D3 M3:M16 AR3:AR7 M18:M25 AR46 A4:C4 Y4:Y11 AG4:AG24 AB62 AB64 Z62 V62 Z64:Z65 V65:W65 AH48:AH49 AH54:AH55 AH62 AH64:AH65 AJ14 AF3:AG3 AJ3:AK3 AJ48:AJ49 AJ54:AJ55 AJ62 AJ64:AJ65 AJ19 AD49:AF49 AD54:AE55 AD62:AE62 AD65:AE65 Z3:Z5 AB4:AB5 AF4:AF5 V21:X21 AB21 AH3:AH9 AD7 AJ4:AJ9 N3:N25 O3:T20 V7:V11 Y13 AD8:AF12 AJ11:AJ12 V13 AD14:AF14 V15 AD16:AE16 AD19:AF21 V19 AJ21 O21:S21 V24 AD24:AF24 M27:N29 AR9:AR28 Z7:Z29 Y15:Y28 E22:L28 AI27:AI29 V27 AD27:AD28 E29 AD30 E31:F31 AB32 AJ31:AJ32 V32:X32 AD32:AF32 H32:L32 AD33 AH11:AH27 AG27 M31:N38 Z31:Z41 AR30:AR38 Y30:Y38 AI31:AI38 E33:F38 AB34 AD34:AF34 AJ34 AD37:AF37 AD35:AD36 V34:X38 V40:W41 AR41 AD38:AD40 E44:F46 AB44:AB45 Z44:Z45 A5:D48 AH29:AH45 AJ41:AJ45 AD41:AE48 AF42:AF48 E47 Z47:Z49 AR49 M44:N49 V44:X49 AI44:AI49 E48:F49 AB47:AB49 AK4:AK55 AC3:AC55 AA8:AA55 AG29:AG55 Y41:Y55 AR51:AR54 O22:T55 O57:T65 Y57:Y61 AG57:AG63 AA57:AA65 AC57:AC64 AK58:AK65 AR62:AR63 Y63:Y65 V64 AG65 AD64 V3:Y3 AD3:AE5 V4:X5 E3:L20 G21:L21 G29:L31 G33:L55 G57:L65">
     <cfRule type="containsBlanks" dxfId="305" priority="281">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ58:AQ60 AQ65">
+  <conditionalFormatting sqref="AR58:AR60 AR65">
     <cfRule type="containsBlanks" dxfId="304" priority="287">
-      <formula>LEN(TRIM(AQ58))=0</formula>
+      <formula>LEN(TRIM(AR58))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17">
@@ -12614,7 +12815,7 @@
       <formula>LEN(TRIM(M26))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:G65 AQ58:AQ60 AQ65 I50:K55 AB50:AB53 Z50:Z53 V50:X53 AD50:AF55 AQ51:AQ54 AA50:AA55 AH50:AJ55 M50:T55 A50:F55 A56:D56 A57:F61 AQ62:AQ63 AB61:AB64 Z61:Z65 V61:X61 AH58:AH65 M57:T65 AI57:AI65 AA57:AA65 I57:K65 A62:E62 V62 V63:X63 AD58:AF63 AJ58:AJ65 V65:X65 V64 AD65:AF65 AD64">
+  <conditionalFormatting sqref="A63:G65 AR58:AR60 AR65 I50:K55 AB50:AB53 Z50:Z53 V50:X53 AD50:AF55 AR51:AR54 AA50:AA55 AH50:AJ55 M50:T55 A50:F55 A56:D56 A57:F61 AR62:AR63 AB61:AB64 Z61:Z65 V61:X61 AH58:AH65 M57:T65 AI57:AI65 AA57:AA65 I57:K65 A62:E62 V62 V63:X63 AD58:AF63 AJ58:AJ65 V65:X65 V64 AD65:AF65 AD64">
     <cfRule type="containsBlanks" dxfId="267" priority="354">
       <formula>LEN(TRIM(A50))=0</formula>
     </cfRule>
@@ -12729,29 +12930,29 @@
       <formula>LEN(TRIM(#REF!))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ42:AQ44">
+  <conditionalFormatting sqref="AR42:AR44">
     <cfRule type="containsBlanks" dxfId="244" priority="253">
-      <formula>LEN(TRIM(AQ42))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ50">
+      <formula>LEN(TRIM(AR42))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR50">
     <cfRule type="containsBlanks" dxfId="243" priority="252">
-      <formula>LEN(TRIM(AQ50))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ55:AQ57">
+      <formula>LEN(TRIM(AR50))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR55:AR57">
     <cfRule type="containsBlanks" dxfId="242" priority="251">
-      <formula>LEN(TRIM(AQ55))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ61">
+      <formula>LEN(TRIM(AR55))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR61">
     <cfRule type="containsBlanks" dxfId="241" priority="250">
-      <formula>LEN(TRIM(AQ61))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ64">
+      <formula>LEN(TRIM(AR61))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR64">
     <cfRule type="containsBlanks" dxfId="240" priority="249">
-      <formula>LEN(TRIM(AQ64))=0</formula>
+      <formula>LEN(TRIM(AR64))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE26:AF26">

</xml_diff>